<commit_message>
More Performance Add Running By Batches
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A074719-4016-460A-8CEA-99650FDD9D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7CBC5A-2D15-4DF3-925A-AAA975F60E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,7 +331,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -389,6 +389,56 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>